<commit_message>
Results of the evaluation in blad 1
</commit_message>
<xml_diff>
--- a/evaluation/evaluationResultsOfficial.xlsx
+++ b/evaluation/evaluationResultsOfficial.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="97">
   <si>
     <t>Course</t>
   </si>
@@ -356,10 +356,13 @@
     <t>Hur viktigt är det att bedöma vilken användargrupp kursen ska riktar sig emot och därefter designa kursen enligt denna bedömning?</t>
   </si>
   <si>
-    <t xml:space="preserve">Hur jag ordsätter användargrupp= målgrupp och studente n = tild deras användare </t>
-  </si>
-  <si>
     <t>Medelvärde</t>
+  </si>
+  <si>
+    <t>Hur viktigt är det att kursen har formativa bedömningar av studenten för att skapa en lärmiljö som ger studenten möjligheter att lära sig i? T.ex. kapiteltester och avslutnings test.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hur jag ordsätter användargrupp= målgrupp och studenten = till deras användare </t>
   </si>
 </sst>
 </file>
@@ -475,8 +478,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="107">
+  <cellStyleXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -668,7 +675,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="107">
+  <cellStyles count="111">
     <cellStyle name="Följd hyperlänk" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Följd hyperlänk" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Följd hyperlänk" xfId="6" builtinId="9" hidden="1"/>
@@ -722,6 +729,8 @@
     <cellStyle name="Följd hyperlänk" xfId="102" builtinId="9" hidden="1"/>
     <cellStyle name="Följd hyperlänk" xfId="104" builtinId="9" hidden="1"/>
     <cellStyle name="Följd hyperlänk" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="110" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlänk" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlänk" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlänk" xfId="5" builtinId="8" hidden="1"/>
@@ -775,6 +784,8 @@
     <cellStyle name="Hyperlänk" xfId="101" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlänk" xfId="103" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlänk" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="109" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3449,7 +3460,7 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3556,7 +3567,7 @@
         <v>74</v>
       </c>
       <c r="I7" s="29" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="36">
@@ -3635,7 +3646,7 @@
     </row>
     <row r="12" spans="1:9" ht="54">
       <c r="A12" s="26" t="s">
-        <v>78</v>
+        <v>95</v>
       </c>
       <c r="B12" t="s">
         <v>59</v>
@@ -3698,11 +3709,12 @@
         <v>71</v>
       </c>
       <c r="C19" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>